<commit_message>
Update the spreadsheets with changes from the python3_updates branch
</commit_message>
<xml_diff>
--- a/data/cci/cci-dataType-ecv-mapping.xlsx
+++ b/data/cci/cci-dataType-ecv-mapping.xlsx
@@ -5,24 +5,24 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies/data/cci/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies2/data/cci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B25B195-96AD-DC44-B5B0-A47056ED5CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B965169-A579-7346-8EAB-D69785667BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{2B508AE5-5675-8647-AEDE-C5A48CC20927}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{4E51E550-2BE2-1645-BA80-54EF4527885D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="115">
   <si>
     <t>dtype URI</t>
   </si>
@@ -349,6 +349,24 @@
   </si>
   <si>
     <t>dtype_pft</t>
+  </si>
+  <si>
+    <t>dtype uncert</t>
+  </si>
+  <si>
+    <t>dtype_vp</t>
+  </si>
+  <si>
+    <t>cciecv_vegParam</t>
+  </si>
+  <si>
+    <t>dtype_wl</t>
+  </si>
+  <si>
+    <t>cciecv_riverDischarge</t>
+  </si>
+  <si>
+    <t>dtype_lcchange</t>
   </si>
 </sst>
 </file>
@@ -358,7 +376,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -394,110 +412,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF9900"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF008000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color rgb="FF666699"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF666699"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF666699"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333399"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF9900"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF993300"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF666699"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -556,8 +470,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,14 +523,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -618,80 +533,8 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFFF"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99CCFF"/>
-        <bgColor rgb="FF99CCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF33CCCC"/>
-        <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF339966"/>
-        <bgColor rgb="FF339966"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF333399"/>
-        <bgColor rgb="FF333399"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF969696"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFCC00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF99CC"/>
-        <bgColor rgb="FFFF99CC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -711,98 +554,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF333399"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF99CCFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF33CCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC0C0C0"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC0C0C0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC0C0C0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC0C0C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF333333"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF333333"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF333333"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF333333"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF333399"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -833,76 +584,80 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="21">
-    <cellStyle name="Accent" xfId="7" xr:uid="{151B587A-EFBE-B347-BAEC-EB8C1192A80A}"/>
-    <cellStyle name="Accent 1" xfId="8" xr:uid="{F4927E1F-54EA-A744-AF66-CE79EB172796}"/>
-    <cellStyle name="Accent 2" xfId="9" xr:uid="{A36EE125-BCCF-F64F-8423-C317432160AA}"/>
-    <cellStyle name="Accent 3" xfId="10" xr:uid="{E1BA9F4A-306C-6B4B-991B-5C1E395574FE}"/>
+  <cellStyles count="22">
+    <cellStyle name="Accent" xfId="7" xr:uid="{D7D7AF64-8052-8247-AB8A-688EB10567E4}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{AEEBC496-539C-D744-9F98-59EB7EDFE846}"/>
+    <cellStyle name="Accent 2" xfId="9" xr:uid="{C090BB5C-0A19-4345-B7ED-40D065E3EFC7}"/>
+    <cellStyle name="Accent 3" xfId="10" xr:uid="{D598C5E8-8617-4D49-810D-F68973E81B5E}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11" xr:uid="{A6877DD5-80E0-4C4F-A171-AA81AC5925FC}"/>
-    <cellStyle name="Excel_BuiltIn_20% - Accent1" xfId="12" xr:uid="{15C8CC18-1BBE-F843-AE63-BEB177DC836C}"/>
-    <cellStyle name="Footnote" xfId="13" xr:uid="{C9D8727C-5077-4249-98AD-D0113B507454}"/>
+    <cellStyle name="Error" xfId="11" xr:uid="{A7CB0392-2D01-2642-8D6D-98B46368B31C}"/>
+    <cellStyle name="Excel_BuiltIn_20% - Accent1" xfId="12" xr:uid="{0F1514B5-7C28-5A4C-A8DD-DFC6E5C40E49}"/>
+    <cellStyle name="Footnote" xfId="13" xr:uid="{8B4DAF32-4553-BD4D-B2CF-2C2E8AD1971B}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="14" xr:uid="{B101D3D1-CCDB-1B4F-8B4C-B6F3675F1DC7}"/>
+    <cellStyle name="Heading" xfId="14" xr:uid="{576D7AD4-2CEA-E249-9F31-80DAF5284E9A}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="15" xr:uid="{CB330D3E-C16B-0F4A-8894-251109F2CA6F}"/>
+    <cellStyle name="Heading1" xfId="15" xr:uid="{42249917-28FF-8747-9378-01DC5BFE789F}"/>
+    <cellStyle name="Hyperlink" xfId="16" xr:uid="{DD868E83-CB47-3941-8BF6-26E19E1D535C}"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="16" xr:uid="{B9261A4B-8CDA-8540-9E5B-32300E770822}"/>
-    <cellStyle name="Result2" xfId="17" xr:uid="{0F264C05-2BA4-CA45-B7A8-00E6FF80FFD3}"/>
-    <cellStyle name="Status" xfId="18" xr:uid="{A7EB5BE2-CFB5-8549-BC49-589CA4B0107A}"/>
-    <cellStyle name="Text" xfId="19" xr:uid="{9D854C5B-184C-644C-BB54-15E4F8026CF5}"/>
-    <cellStyle name="Warning" xfId="20" xr:uid="{5ED47CB5-2993-F040-BBAF-C59E2AF9A39E}"/>
+    <cellStyle name="Result" xfId="17" xr:uid="{E9D0D85E-1670-2B4A-BA13-FD58272D8396}"/>
+    <cellStyle name="Result2" xfId="18" xr:uid="{4E1EB7BB-A033-0742-93A6-E13C9A94B8EE}"/>
+    <cellStyle name="Status" xfId="19" xr:uid="{8241E3CA-34EA-0B4C-814B-4DE891DDBDD0}"/>
+    <cellStyle name="Text" xfId="20" xr:uid="{5E50CFBD-0418-4C45-9A47-16D8AE70F978}"/>
+    <cellStyle name="Warning" xfId="21" xr:uid="{EE1CB5F0-0CB9-C044-8A49-D032CFB9B6E6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1233,18 +988,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB01D6C7-04F9-9C41-B539-EE5291CB1A53}">
-  <dimension ref="A1:D85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03066BF4-F4E8-0F4A-A490-1A16D2F31AC9}">
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="8" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="64" width="13.33203125" customWidth="1"/>
+    <col min="65" max="65" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -2434,6 +2190,62 @@
         <v>37</v>
       </c>
       <c r="D85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A86" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>37</v>
+      </c>
+      <c r="D86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>111</v>
+      </c>
+      <c r="D87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A88" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>113</v>
+      </c>
+      <c r="D88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" t="s">
+        <v>37</v>
+      </c>
+      <c r="D89" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2444,12 +2256,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B8E626-5E58-4B4F-B17C-0A0EBED79EE5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46DDE75-9958-0C45-BAFA-DD843224779E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1023" width="13.33203125" customWidth="1"/>
     <col min="1024" max="1024" width="10.6640625" customWidth="1"/>
@@ -2460,12 +2272,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DB9E79-952B-6B42-ABCB-34E6B0D32C56}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81E7961-87F9-A342-B62A-695DB85B165D}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1023" width="13.33203125" customWidth="1"/>
     <col min="1024" max="1024" width="10.6640625" customWidth="1"/>

</xml_diff>

<commit_message>
add dataType ECV mapping
</commit_message>
<xml_diff>
--- a/data/cci/cci-dataType-ecv-mapping.xlsx
+++ b/data/cci/cci-dataType-ecv-mapping.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies2/data/cci/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies/data/cci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B965169-A579-7346-8EAB-D69785667BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988F0833-324E-A94E-ADCC-47810A45B928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{4E51E550-2BE2-1645-BA80-54EF4527885D}"/>
+    <workbookView xWindow="-55840" yWindow="-1560" windowWidth="30240" windowHeight="18880" xr2:uid="{4E51E550-2BE2-1645-BA80-54EF4527885D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -351,9 +351,6 @@
     <t>dtype_pft</t>
   </si>
   <si>
-    <t>dtype uncert</t>
-  </si>
-  <si>
     <t>dtype_vp</t>
   </si>
   <si>
@@ -367,6 +364,9 @@
   </si>
   <si>
     <t>dtype_lcchange</t>
+  </si>
+  <si>
+    <t>dtype_uncert</t>
   </si>
 </sst>
 </file>
@@ -616,24 +616,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Accent" xfId="7" xr:uid="{D7D7AF64-8052-8247-AB8A-688EB10567E4}"/>
@@ -991,11 +987,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03066BF4-F4E8-0F4A-A490-1A16D2F31AC9}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" style="8" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
@@ -1003,7 +1001,7 @@
     <col min="65" max="65" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1017,1030 +1015,1030 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="6" t="s">
+      <c r="B72" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D72" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
+      <c r="D72" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="6" t="s">
+      <c r="B73" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+      <c r="D73" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B74" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="6" t="s">
+      <c r="B74" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A75" s="8" t="s">
+      <c r="D74" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>30</v>
       </c>
       <c r="B75" t="s">
@@ -2053,8 +2051,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="8" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>94</v>
       </c>
       <c r="B76" t="s">
@@ -2067,8 +2065,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>96</v>
       </c>
       <c r="B77" t="s">
@@ -2081,8 +2079,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="8" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>98</v>
       </c>
       <c r="B78" t="s">
@@ -2095,8 +2093,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="8" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>99</v>
       </c>
       <c r="B79" t="s">
@@ -2109,8 +2107,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A80" s="8" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>100</v>
       </c>
       <c r="B80" t="s">
@@ -2123,8 +2121,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>102</v>
       </c>
       <c r="B81" t="s">
@@ -2137,8 +2135,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="8" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>103</v>
       </c>
       <c r="B82" t="s">
@@ -2151,8 +2149,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>104</v>
       </c>
       <c r="B83" t="s">
@@ -2165,7 +2163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>106</v>
       </c>
@@ -2179,8 +2177,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>108</v>
       </c>
       <c r="B85" t="s">
@@ -2193,9 +2191,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A86" s="8" t="s">
-        <v>109</v>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>114</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
@@ -2207,37 +2205,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="8" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>109</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
         <v>110</v>
       </c>
-      <c r="B87" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>111</v>
       </c>
-      <c r="D87" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="8" t="s">
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
         <v>112</v>
       </c>
-      <c r="B88" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>113</v>
-      </c>
-      <c r="D88" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="B89" t="s">
         <v>5</v>
@@ -2261,7 +2259,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1023" width="13.33203125" customWidth="1"/>
     <col min="1024" max="1024" width="10.6640625" customWidth="1"/>
@@ -2277,7 +2275,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1023" width="13.33203125" customWidth="1"/>
     <col min="1024" max="1024" width="10.6640625" customWidth="1"/>

</xml_diff>